<commit_message>
update db init + add MySQL enums
</commit_message>
<xml_diff>
--- a/config/data_microscopes.xlsx
+++ b/config/data_microscopes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Stage\Referencement-Microscopes-ReMiSoL\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBFE361-D91F-43BD-9E6C-8CE8CD16517E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0EE5ED-76EC-49A0-8618-861A4284BEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15720" xr2:uid="{0E5F2783-0881-4071-B044-90982E8746C1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="80">
   <si>
     <t>société</t>
   </si>
@@ -212,6 +212,69 @@
   </si>
   <si>
     <t>Brand</t>
+  </si>
+  <si>
+    <t>NanoDrive</t>
+  </si>
+  <si>
+    <t>Vortis1</t>
+  </si>
+  <si>
+    <t>Vortis2</t>
+  </si>
+  <si>
+    <t>Vortis2.1</t>
+  </si>
+  <si>
+    <t>NanoWizard 5</t>
+  </si>
+  <si>
+    <t>PX Ultra Controller</t>
+  </si>
+  <si>
+    <t>BL222TNTF Tower</t>
+  </si>
+  <si>
+    <t>BL222RNTF Ratiopac Pro</t>
+  </si>
+  <si>
+    <t>Ntegra II</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>Next II</t>
+  </si>
+  <si>
+    <t>Scienta Omicron</t>
+  </si>
+  <si>
+    <t>Omicron</t>
+  </si>
+  <si>
+    <t>STM1</t>
+  </si>
+  <si>
+    <t>Matrix 3.X</t>
+  </si>
+  <si>
+    <t>STM2</t>
+  </si>
+  <si>
+    <t>Matrix 4.X</t>
+  </si>
+  <si>
+    <t>SPM Probe</t>
+  </si>
+  <si>
+    <t>Nanonis</t>
+  </si>
+  <si>
+    <t>Zurich</t>
+  </si>
+  <si>
+    <t>GXSM</t>
   </si>
 </sst>
 </file>
@@ -563,17 +626,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2088B183-177B-491F-A2E5-89C3A5ADE5F7}">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="I21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="29.5703125" customWidth="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1"/>
-    <col min="8" max="8" width="48.28515625" customWidth="1"/>
+    <col min="8" max="8" width="51" customWidth="1"/>
     <col min="9" max="9" width="63.140625" customWidth="1"/>
     <col min="10" max="10" width="69.28515625" customWidth="1"/>
     <col min="11" max="11" width="75.28515625" customWidth="1"/>
@@ -618,199 +681,130 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2" t="str">
-        <f>"insert into compagny values("&amp;G2&amp;", '"&amp;$A$2&amp;"');"</f>
-        <v>insert into compagny values(1, 'Bruker');</v>
+        <f>"insert into compagny values(NULL, '"&amp;$A$2&amp;"');"</f>
+        <v>insert into compagny values(NULL, 'Bruker');</v>
       </c>
       <c r="I2" t="str">
-        <f>"insert into brand values("&amp;G2&amp;", '"&amp;B2&amp;"',"&amp;$G$2&amp;");"</f>
-        <v>insert into brand values(1, 'Bruker',1);</v>
+        <f>"insert into brand values(NULL, '"&amp;B2&amp;"',1);"</f>
+        <v>insert into brand values(NULL, 'Bruker',1);</v>
       </c>
       <c r="J2" t="str">
-        <f>"insert into model values("&amp;G2&amp;", '"&amp;C2&amp;"',"&amp;$G$2&amp;");"</f>
-        <v>insert into model values(1, 'multimode',1);</v>
+        <f>"insert into model values(NULL, '"&amp;C2&amp;"',1);"</f>
+        <v>insert into model values(NULL, 'multimode',1);</v>
       </c>
       <c r="K2" t="str">
-        <f>"insert into controller values("&amp;G2&amp;", '"&amp;D2&amp;"',"&amp;$G$2&amp;");"</f>
-        <v>insert into controller values(1, 'Nanoscope IIIa',1);</v>
+        <f>"insert into controller values(NULL, '"&amp;D2&amp;"',1);"</f>
+        <v>insert into controller values(NULL, 'Nanoscope IIIa',1);</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="I3" t="str">
-        <f>"insert into brand values("&amp;G3&amp;", '"&amp;B12&amp;"',"&amp;$G$2&amp;");"</f>
-        <v>insert into brand values(2, 'JPK',1);</v>
-      </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J14" si="0">"insert into model values("&amp;G3&amp;", '"&amp;C3&amp;"',"&amp;$G$2&amp;");"</f>
-        <v>insert into model values(2, 'dimension 3000',1);</v>
+        <f t="shared" ref="J3:J12" si="0">"insert into model values(NULL, '"&amp;C3&amp;"',1);"</f>
+        <v>insert into model values(NULL, 'dimension 3000',1);</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K5" si="1">"insert into controller values("&amp;G3&amp;", '"&amp;D3&amp;"',"&amp;$G$2&amp;");"</f>
-        <v>insert into controller values(2, 'Nanoscope Quadrex',1);</v>
+        <f t="shared" ref="K3:K11" si="1">"insert into controller values(NULL, '"&amp;D3&amp;"',1);"</f>
+        <v>insert into controller values(NULL, 'Nanoscope Quadrex',1);</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
       <c r="J4" t="str">
         <f t="shared" si="0"/>
-        <v>insert into model values(3, 'dimension 3100',1);</v>
+        <v>insert into model values(NULL, 'dimension 3100',1);</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="1"/>
-        <v>insert into controller values(3, 'Nanoscope V',1);</v>
+        <v>insert into controller values(NULL, 'Nanoscope V',1);</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
       <c r="J5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into model values(4, 'dimension Icon',1);</v>
+        <v>insert into model values(NULL, 'dimension Icon',1);</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="1"/>
-        <v>insert into controller values(4, 'Nanoscope 6',1);</v>
+        <v>insert into controller values(NULL, 'Nanoscope 6',1);</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="G6">
-        <v>5</v>
+      <c r="D6" t="s">
+        <v>59</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
-        <v>insert into model values(5, 'Edge',1);</v>
+        <v>insert into model values(NULL, 'Edge',1);</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into controller values(NULL, 'NanoDrive',1);</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
       <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="G7">
-        <v>6</v>
-      </c>
       <c r="J7" t="str">
         <f t="shared" si="0"/>
-        <v>insert into model values(6, 'dimension XR',1);</v>
+        <v>insert into model values(NULL, 'dimension XR',1);</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
       <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="G8">
-        <v>7</v>
-      </c>
       <c r="J8" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into model values(7, 'dimension FastScan',1);</v>
+        <f>"insert into model values(NULL, '"&amp;C8&amp;"',1);"</f>
+        <v>insert into model values(NULL, 'dimension FastScan',1);</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
       <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="G9">
-        <v>8</v>
-      </c>
       <c r="J9" t="str">
         <f t="shared" si="0"/>
-        <v>insert into model values(8, 'dimension Icon Raman',1);</v>
+        <v>insert into model values(NULL, 'dimension Icon Raman',1);</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
       <c r="C10" t="s">
         <v>21</v>
       </c>
-      <c r="G10">
-        <v>9</v>
-      </c>
       <c r="J10" t="str">
         <f t="shared" si="0"/>
-        <v>insert into model values(9, 'MultiMode 8 HR',1);</v>
+        <v>insert into model values(NULL, 'MultiMode 8 HR',1);</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
       <c r="C11" t="s">
         <v>22</v>
       </c>
-      <c r="G11">
-        <v>10</v>
-      </c>
       <c r="J11" t="str">
         <f t="shared" si="0"/>
-        <v>insert into model values(10, 'Innova',1);</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12">
-        <v>11</v>
-      </c>
-      <c r="J12" t="str">
-        <f>"insert into model values("&amp;G12&amp;", '"&amp;C12&amp;"',"&amp;2&amp;");"</f>
-        <v>insert into model values(11, 'Nanowizard',2);</v>
+        <v>insert into model values(NULL, 'Innova',1);</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -818,271 +812,478 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" t="str">
+        <f>"insert into brand values(NULL, '"&amp;B13&amp;"',1);"</f>
+        <v>insert into brand values(NULL, 'JPK',1);</v>
+      </c>
+      <c r="J13" t="str">
+        <f>"insert into model values(NULL, '"&amp;C13&amp;"',2);"</f>
+        <v>insert into model values(NULL, 'Nanowizard',2);</v>
+      </c>
+      <c r="K13" t="str">
+        <f>"insert into controller values(NULL, '"&amp;D13&amp;"',2);"</f>
+        <v>insert into controller values(NULL, 'Vortis1',2);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
         <v>18</v>
       </c>
-      <c r="G13">
-        <v>12</v>
-      </c>
-      <c r="J13" t="str">
-        <f t="shared" ref="J13:J14" si="2">"insert into model values("&amp;G13&amp;", '"&amp;C13&amp;"',"&amp;2&amp;");"</f>
-        <v>insert into model values(12, 'NanoWizard NanoOptics',2);</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" t="str">
+        <f>"insert into model values(NULL, '"&amp;C14&amp;"',2);"</f>
+        <v>insert into model values(NULL, 'NanoWizard NanoOptics',2);</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" ref="K14:K15" si="2">"insert into controller values(NULL, '"&amp;D14&amp;"',2);"</f>
+        <v>insert into controller values(NULL, 'Vortis2',2);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s">
+        <v>62</v>
+      </c>
+      <c r="J15" t="str">
+        <f>"insert into model values(NULL, '"&amp;C15&amp;"',2);"</f>
+        <v>insert into model values(NULL, 'NanoWizard 5',2);</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into controller values(NULL, 'Vortis2.1',2);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
         <v>19</v>
       </c>
-      <c r="G14">
-        <v>13</v>
-      </c>
-      <c r="J14" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into model values(13, 'NanoWizard 4 XP NanoScience',2);</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="J16" t="str">
+        <f>"insert into model values(NULL, '"&amp;C16&amp;"',2);"</f>
+        <v>insert into model values(NULL, 'NanoWizard 4 XP NanoScience',2);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>23</v>
       </c>
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16">
-        <v>15</v>
-      </c>
-      <c r="H16" t="str">
-        <f>"insert into compagny values("&amp;2&amp;", '"&amp;$A$16&amp;"');"</f>
-        <v>insert into compagny values(2, 'Oxford Instrument');</v>
-      </c>
-      <c r="I16" t="str">
-        <f>"insert into brand values("&amp;3&amp;", '"&amp;B16&amp;"',"&amp;2&amp;");"</f>
-        <v>insert into brand values(3, 'Asylum Research',2);</v>
-      </c>
-      <c r="J16" t="str">
-        <f>"insert into model values("&amp;G16&amp;", '"&amp;C16&amp;"',"&amp;3&amp;");"</f>
-        <v>insert into model values(15, 'MFP3D origin',3);</v>
-      </c>
-      <c r="K16" t="str">
-        <f>"insert into controller values("&amp;G16&amp;", '"&amp;D16&amp;"',"&amp;2&amp;");"</f>
-        <v>insert into controller values(15, 'ARC2',2);</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17">
-        <v>16</v>
-      </c>
-      <c r="J17" t="str">
-        <f t="shared" ref="J17:J23" si="3">"insert into model values("&amp;G17&amp;", '"&amp;C17&amp;"',"&amp;3&amp;");"</f>
-        <v>insert into model values(16, 'MFP3D Infinity',3);</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>24</v>
       </c>
       <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" t="str">
+        <f>"insert into compagny values(NULL, '"&amp;A18&amp;"');"</f>
+        <v>insert into compagny values(NULL, 'Oxford Instrument');</v>
+      </c>
+      <c r="I18" t="str">
+        <f>"insert into brand values(NULL, '"&amp;B18&amp;"',2);"</f>
+        <v>insert into brand values(NULL, 'Asylum Research',2);</v>
+      </c>
+      <c r="J18" t="str">
+        <f>"insert into model values(NULL, '"&amp;C18&amp;"',3);"</f>
+        <v>insert into model values(NULL, 'MFP3D origin',3);</v>
+      </c>
+      <c r="K18" t="str">
+        <f>"insert into controller values(NULL, '"&amp;D18&amp;"',3);"</f>
+        <v>insert into controller values(NULL, 'ARC2',3);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" ref="J19:J25" si="3">"insert into model values(NULL, '"&amp;C19&amp;"',3);"</f>
+        <v>insert into model values(NULL, 'MFP3D Infinity',3);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
         <v>28</v>
-      </c>
-      <c r="G18">
-        <v>17</v>
-      </c>
-      <c r="J18" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into model values(17, 'MFP3D Bio',3);</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19">
-        <v>18</v>
-      </c>
-      <c r="J19" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into model values(18, 'Cypher S',3);</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20">
-        <v>19</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="3"/>
-        <v>insert into model values(19, 'Cypher ES',3);</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
+        <v>insert into model values(NULL, 'MFP3D Bio',3);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>31</v>
-      </c>
-      <c r="G21">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="3"/>
-        <v>insert into model values(20, 'Cypher ES polymer',3);</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>24</v>
-      </c>
+        <v>insert into model values(NULL, 'Cypher S',3);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>32</v>
-      </c>
-      <c r="G22">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="3"/>
-        <v>insert into model values(21, 'Cypher VRS',3);</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>24</v>
-      </c>
+        <v>insert into model values(NULL, 'Cypher ES',3);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>33</v>
-      </c>
-      <c r="G23">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="3"/>
-        <v>insert into model values(22, 'Jupiter XR',3);</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+        <v>insert into model values(NULL, 'Cypher ES polymer',3);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into model values(NULL, 'Cypher VRS',3);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into model values(NULL, 'Jupiter XR',3);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>34</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B27" t="s">
         <v>35</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C27" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
+      <c r="H27" t="str">
+        <f t="shared" ref="H19:H56" si="4">"insert into compagny values(NULL, '"&amp;A27&amp;"');"</f>
+        <v>insert into compagny values(NULL, 'Park Systems');</v>
+      </c>
+      <c r="I27" t="str">
+        <f>"insert into brand values(NULL, '"&amp;B27&amp;"',3);"</f>
+        <v>insert into brand values(NULL, 'Park System',3);</v>
+      </c>
+      <c r="J27" t="str">
+        <f>"insert into model values(NULL, '"&amp;C27&amp;"',4);"</f>
+        <v>insert into model values(NULL, 'XE',4);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
+      <c r="J28" t="str">
+        <f t="shared" ref="J28:J29" si="5">"insert into model values(NULL, '"&amp;C28&amp;"',4);"</f>
+        <v>insert into model values(NULL, 'FX',4);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="J29" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into model values(NULL, 'NX',4);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>39</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>39</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C31" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
+      <c r="H31" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into compagny values(NULL, 'NanoSurf');</v>
+      </c>
+      <c r="I31" t="str">
+        <f>"insert into brand values(NULL, '"&amp;B31&amp;"',4);"</f>
+        <v>insert into brand values(NULL, 'NanoSurf',4);</v>
+      </c>
+      <c r="J31" t="str">
+        <f>"insert into model values(NULL, '"&amp;C31&amp;"',5);"</f>
+        <v>insert into model values(NULL, 'NaioAFM',5);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+      <c r="J32" t="str">
+        <f t="shared" ref="J32:J35" si="6">"insert into model values(NULL, '"&amp;C32&amp;"',5);"</f>
+        <v>insert into model values(NULL, 'NaioSTM',5);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
+      <c r="J33" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into model values(NULL, 'DriveAFM',5);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+      <c r="J34" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into model values(NULL, 'FlexAFM',5);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="J35" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into model values(NULL, 'CoreAFM',5);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>45</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B37" t="s">
         <v>46</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C37" t="s">
         <v>47</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D37" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+      <c r="H37" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into compagny values(NULL, 'Scientec');</v>
+      </c>
+      <c r="I37" t="str">
+        <f>"insert into brand values(NULL, '"&amp;B37&amp;"',5);"</f>
+        <v>insert into brand values(NULL, 'CSI',5);</v>
+      </c>
+      <c r="J37" t="str">
+        <f>"insert into model values(NULL, '"&amp;C37&amp;"',6);"</f>
+        <v>insert into model values(NULL, 'NanoObserver',6);</v>
+      </c>
+      <c r="K37" t="str">
+        <f>"insert into controller values(NULL, '"&amp;D37&amp;"',6);"</f>
+        <v>insert into controller values(NULL, 'Galaxy Dual controller',6);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C37">
+      <c r="J38" t="str">
+        <f t="shared" ref="J38:J42" si="7">"insert into model values(NULL, '"&amp;C38&amp;"',6);"</f>
+        <v>insert into model values(NULL, 'Resiscope',6);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C39">
         <v>5100</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C38">
+      <c r="J39" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into model values(NULL, '5100',6);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C40">
         <v>5500</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="J40" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into model values(NULL, '5500',6);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>50</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C42" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
+      <c r="D42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into compagny values(NULL, 'NT-MDT');</v>
+      </c>
+      <c r="I42" t="str">
+        <f>"insert into brand values(NULL, '"&amp;B42&amp;"',6);"</f>
+        <v>insert into brand values(NULL, '',6);</v>
+      </c>
+      <c r="J42" t="str">
+        <f>"insert into model values(NULL, '"&amp;C42&amp;"',7);"</f>
+        <v>insert into model values(NULL, 'Ntegra',7);</v>
+      </c>
+      <c r="K42" t="str">
+        <f>"insert into controller values(NULL, '"&amp;D42&amp;"',7);"</f>
+        <v>insert into controller values(NULL, 'PX Ultra Controller',7);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
+      <c r="D43" t="s">
+        <v>65</v>
+      </c>
+      <c r="J43" t="str">
+        <f t="shared" ref="J43:J48" si="8">"insert into model values(NULL, '"&amp;C43&amp;"',7);"</f>
+        <v>insert into model values(NULL, 'Ntegra NanoIR',7);</v>
+      </c>
+      <c r="K43" t="str">
+        <f t="shared" ref="K43:K44" si="9">"insert into controller values(NULL, '"&amp;D43&amp;"',7);"</f>
+        <v>insert into controller values(NULL, 'BL222TNTF Tower',7);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
+      <c r="D44" t="s">
+        <v>66</v>
+      </c>
+      <c r="J44" t="str">
+        <f t="shared" si="8"/>
+        <v>insert into model values(NULL, 'Vega',7);</v>
+      </c>
+      <c r="K44" t="str">
+        <f t="shared" si="9"/>
+        <v>insert into controller values(NULL, 'BL222RNTF Ratiopac Pro',7);</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
         <v>54</v>
+      </c>
+      <c r="J45" t="str">
+        <f t="shared" si="8"/>
+        <v>insert into model values(NULL, 'Solver',7);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>67</v>
+      </c>
+      <c r="J46" t="str">
+        <f t="shared" si="8"/>
+        <v>insert into model values(NULL, 'Ntegra II',7);</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>68</v>
+      </c>
+      <c r="J47" t="str">
+        <f t="shared" si="8"/>
+        <v>insert into model values(NULL, 'Next',7);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>69</v>
+      </c>
+      <c r="J48" t="str">
+        <f t="shared" si="8"/>
+        <v>insert into model values(NULL, 'Next II',7);</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" t="s">
+        <v>71</v>
+      </c>
+      <c r="C50" t="s">
+        <v>72</v>
+      </c>
+      <c r="D50" t="s">
+        <v>73</v>
+      </c>
+      <c r="H50" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into compagny values(NULL, 'Scienta Omicron');</v>
+      </c>
+      <c r="I50" t="str">
+        <f>"insert into brand values(NULL, '"&amp;B50&amp;"',7);"</f>
+        <v>insert into brand values(NULL, 'Omicron',7);</v>
+      </c>
+      <c r="J50" t="str">
+        <f>"insert into model values(NULL, '"&amp;C50&amp;"',8);"</f>
+        <v>insert into model values(NULL, 'STM1',8);</v>
+      </c>
+      <c r="K50" t="str">
+        <f>"insert into controller values(NULL, '"&amp;D50&amp;"',8);"</f>
+        <v>insert into controller values(NULL, 'Matrix 3.X',8);</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>74</v>
+      </c>
+      <c r="D51" t="s">
+        <v>75</v>
+      </c>
+      <c r="J51" t="str">
+        <f t="shared" ref="J51:J52" si="10">"insert into model values(NULL, '"&amp;C51&amp;"',8);"</f>
+        <v>insert into model values(NULL, 'STM2',8);</v>
+      </c>
+      <c r="K51" t="str">
+        <f>"insert into controller values(NULL, '"&amp;D51&amp;"',8);"</f>
+        <v>insert into controller values(NULL, 'Matrix 4.X',8);</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>76</v>
+      </c>
+      <c r="J52" t="str">
+        <f t="shared" si="10"/>
+        <v>insert into model values(NULL, 'SPM Probe',8);</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>